<commit_message>
node v4.0.* 版本window 64 linux 64位编译
</commit_message>
<xml_diff>
--- a/test/嵌套循环例子.xlsx
+++ b/test/嵌套循环例子.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>&lt;%=_data_[0][0].table_name%&gt;</t>
   </si>
@@ -99,15 +99,11 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;%forREnd(1)%&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;%=rs2.cb1+" / "+rs2.bn1%&gt;</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;%forREnd(9)%&gt;</t>
+    <t>&lt;%forREnd%&gt;</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1094,7 +1090,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="29"/>
@@ -1104,7 +1100,7 @@
     </row>
     <row r="8" spans="1:17" ht="21" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="10" t="s">
@@ -1162,7 +1158,7 @@
     </row>
     <row r="12" spans="1:17" ht="18.95" customHeight="1">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="17"/>
     </row>

</xml_diff>